<commit_message>
fix punto repetido rubrica
</commit_message>
<xml_diff>
--- a/contenido/TrabajoFinal/2022-rubrica-frontend-smu.xlsx
+++ b/contenido/TrabajoFinal/2022-rubrica-frontend-smu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9335"/>
+    <workbookView windowWidth="28800" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Rubrica" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Puntaje Total</t>
   </si>
@@ -239,11 +239,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.0"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -311,8 +311,108 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,24 +426,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,91 +442,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,13 +470,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,163 +650,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,7 +688,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -701,9 +703,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -733,33 +733,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -796,11 +774,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -813,160 +804,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -979,14 +979,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -995,75 +991,76 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1272,19 +1269,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:H955"/>
+  <dimension ref="B1:H954"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:H3"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="4.75" customWidth="1"/>
+    <col min="2" max="2" width="4.75333333333333" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="7" width="29.625" customWidth="1"/>
-    <col min="8" max="8" width="14.3833333333333" customWidth="1"/>
+    <col min="4" max="7" width="29.6266666666667" customWidth="1"/>
+    <col min="8" max="8" width="14.38" customWidth="1"/>
     <col min="9" max="26" width="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1293,8 +1290,8 @@
         <v>0</v>
       </c>
       <c r="D1" s="2">
-        <f>16*4</f>
-        <v>64</v>
+        <f>+MAX(B8:B99)*4</f>
+        <v>60</v>
       </c>
     </row>
     <row r="2" ht="36" customHeight="1" spans="2:8">
@@ -1303,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <f>SUM(H8:H18)</f>
+        <f>SUM(H8:H17)</f>
         <v>0</v>
       </c>
       <c r="E2" s="1"/>
@@ -1340,411 +1337,406 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" ht="36" customHeight="1" spans="2:8">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" ht="36" customHeight="1" spans="2:8">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="16"/>
     </row>
-    <row r="8" ht="43.2" spans="2:8">
-      <c r="B8" s="14">
+    <row r="8" ht="47.25" spans="2:8">
+      <c r="B8" s="11">
+        <f>+IF(ISNUMBER(B7),B7+1,IF(ISNUMBER(B6),B6+1,1))</f>
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="17"/>
     </row>
     <row r="9" ht="81.75" customHeight="1" spans="2:8">
-      <c r="B9" s="14">
+      <c r="B9" s="11">
+        <f>+IF(ISNUMBER(B8),B8+1,IF(ISNUMBER(B7),B7+1,1))</f>
         <v>2</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" ht="66" customHeight="1" spans="2:8">
-      <c r="B10" s="18">
+    <row r="10" ht="73" customHeight="1" spans="2:8">
+      <c r="B10" s="11">
+        <f>+IF(ISNUMBER(#REF!),#REF!+1,IF(ISNUMBER(B9),B9+1,1))</f>
         <v>3</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>20</v>
+      <c r="C10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" ht="73" customHeight="1" spans="2:8">
-      <c r="B11" s="18">
+    <row r="11" ht="77" customHeight="1" spans="2:8">
+      <c r="B11" s="11">
+        <f>+IF(ISNUMBER(B10),B10+1,IF(ISNUMBER(#REF!),#REF!+1,1))</f>
         <v>4</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>25</v>
+      <c r="C11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" ht="77" customHeight="1" spans="2:8">
-      <c r="B12" s="18">
+    <row r="12" ht="36" customHeight="1" spans="2:8">
+      <c r="B12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" ht="78.75" spans="2:8">
+      <c r="B13" s="11">
+        <f t="shared" ref="B13:B17" si="0">+IF(ISNUMBER(B12),B12+1,IF(ISNUMBER(B11),B11+1,1))</f>
         <v>5</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="17"/>
+      <c r="C13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="17"/>
     </row>
-    <row r="13" ht="36" customHeight="1" spans="2:8">
-      <c r="B13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" ht="72" spans="2:8">
-      <c r="B14" s="18">
+    <row r="14" ht="63" spans="2:8">
+      <c r="B14" s="11">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="C14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="13" t="s">
         <v>36</v>
       </c>
       <c r="H14" s="17"/>
     </row>
-    <row r="15" ht="57.6" spans="2:8">
-      <c r="B15" s="18">
+    <row r="15" ht="45" customHeight="1" spans="2:8">
+      <c r="B15" s="11">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>36</v>
+      <c r="C15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" ht="45" customHeight="1" spans="2:8">
-      <c r="B16" s="18">
+    <row r="16" ht="78.75" spans="2:8">
+      <c r="B16" s="11">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>43</v>
+      <c r="C16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="H16" s="17"/>
     </row>
-    <row r="17" ht="72" spans="2:8">
-      <c r="B17" s="18">
+    <row r="17" ht="47.25" spans="2:8">
+      <c r="B17" s="11">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>30</v>
+      <c r="C17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" ht="43.2" spans="2:8">
-      <c r="B18" s="18">
+    <row r="18" ht="36" customHeight="1" spans="2:8">
+      <c r="B18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" ht="47.25" spans="2:8">
+      <c r="B19" s="11">
+        <f t="shared" ref="B19:B22" si="1">+IF(ISNUMBER(B18),B18+1,IF(ISNUMBER(B17),B17+1,1))</f>
         <v>10</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="16" t="s">
+      <c r="C19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="17"/>
+      <c r="H19" s="17"/>
     </row>
-    <row r="19" ht="36" customHeight="1" spans="2:8">
-      <c r="B19" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" ht="43.2" spans="2:8">
-      <c r="B20" s="18">
+    <row r="20" ht="96" customHeight="1" spans="2:8">
+      <c r="B20" s="11">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>36</v>
+      <c r="C20" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" ht="96" customHeight="1" spans="2:8">
-      <c r="B21" s="18">
+    <row r="21" ht="74" customHeight="1" spans="2:8">
+      <c r="B21" s="11">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>30</v>
+      <c r="C21" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" ht="74" customHeight="1" spans="2:8">
-      <c r="B22" s="18">
+    <row r="22" ht="126" spans="2:8">
+      <c r="B22" s="11">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="16" t="s">
+      <c r="C22" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="13" t="s">
         <v>36</v>
       </c>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" ht="100.8" spans="2:8">
-      <c r="B23" s="18">
+    <row r="23" ht="36" customHeight="1" spans="2:8">
+      <c r="B23" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" ht="94.5" spans="2:8">
+      <c r="B24" s="11">
+        <f>+IF(ISNUMBER(B23),B23+1,IF(ISNUMBER(B22),B22+1,1))</f>
         <v>14</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="16" t="s">
+      <c r="C24" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F24" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G24" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="17"/>
+      <c r="H24" s="17"/>
     </row>
-    <row r="24" ht="36" customHeight="1" spans="2:8">
-      <c r="B24" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
-    </row>
-    <row r="25" ht="86.4" spans="2:8">
-      <c r="B25" s="18">
+    <row r="25" ht="36" customHeight="1" spans="2:8">
+      <c r="B25" s="11">
+        <f>+IF(ISNUMBER(B24),B24+1,IF(ISNUMBER(B23),B23+1,1))</f>
         <v>15</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>36</v>
+      <c r="C25" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="H25" s="17"/>
     </row>
-    <row r="26" ht="36" customHeight="1" spans="2:8">
-      <c r="B26" s="18">
-        <v>16</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="17"/>
-    </row>
+    <row r="26" ht="36" customHeight="1"/>
     <row r="27" ht="36" customHeight="1"/>
     <row r="28" ht="36" customHeight="1"/>
     <row r="29" ht="36" customHeight="1"/>
@@ -2673,15 +2665,14 @@
     <row r="952" ht="36" customHeight="1"/>
     <row r="953" ht="36" customHeight="1"/>
     <row r="954" ht="36" customHeight="1"/>
-    <row r="955" ht="36" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="landscape"/>

</xml_diff>